<commit_message>
Añadido final de documentación en español asi como su contraparte en Inglés, así como un README
</commit_message>
<xml_diff>
--- a/Documentación/Desglose Gastos.xlsx
+++ b/Documentación/Desglose Gastos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\warri\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\warri\OneDrive\Documentos\Escuela\ComputaciónGráfica\Práctica7\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2363E13A-053A-439C-867A-04132DE24FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F361030-3255-41C4-A250-3350CB13957A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9564739D-0355-4062-9325-BCCD58C55580}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Disipador CPU Cooler Master 212 Led</t>
   </si>
   <si>
-    <t>Fuende te poder EVGA 450 Bronce 80 Plus 24-pin ATX</t>
-  </si>
-  <si>
     <t>16 Gb Ram Cosair Vengeance</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>Utilidades descontando impuestos</t>
+  </si>
+  <si>
+    <t>Fuente de poder EVGA 450 Bronce 80 Plus 24-pin ATX</t>
   </si>
 </sst>
 </file>
@@ -155,7 +155,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -292,30 +292,30 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +633,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,202 +652,202 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2"/>
+      <c r="A3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4569</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4">
-        <v>4569</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1500</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="3">
-        <v>5</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1500</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>6</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>120</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>6</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <f xml:space="preserve"> F9/I6</f>
         <v>3.1666666666666665</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3">
+        <v>569</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F8" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4">
-        <v>569</v>
-      </c>
-      <c r="E8" s="3" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3">
+        <v>989</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4">
-        <v>989</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="17">
+      <c r="F9" s="13">
         <f>SUM(F5:F8)</f>
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1608</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2879</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3">
+        <v>300</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4">
-        <v>1608</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="4">
-        <v>2879</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="4">
-        <v>300</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>800</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="E13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="6">
         <f xml:space="preserve"> PRODUCT(B16,F9)</f>
         <v>5574.2833333333328</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3">
         <v>3889</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="6">
         <f xml:space="preserve"> PRODUCT(F9,H6)</f>
         <v>2280</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="14">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="10">
         <f>SUM(B5:B14)</f>
         <v>17603</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="15">
+      <c r="E15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="11">
         <f xml:space="preserve"> SUM(F13:F14)</f>
         <v>7854.2833333333328</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="6">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5">
         <f xml:space="preserve"> (B15 /12) /5</f>
         <v>293.38333333333333</v>
       </c>
@@ -856,75 +856,75 @@
       <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="13"/>
+      <c r="A18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="17"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>200</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4">
-        <v>200</v>
-      </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>1500</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="14">
+      <c r="A22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="10">
         <f xml:space="preserve"> SUM(B19:B21)</f>
         <v>2300</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="13"/>
+      <c r="A25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="6">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="5">
         <f xml:space="preserve"> (F15 ) - SUM(B22)</f>
         <v>5554.2833333333328</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="9">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="8">
         <f xml:space="preserve"> B26 * 0.025</f>
         <v>138.85708333333332</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="10">
+      <c r="A28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="9">
         <f xml:space="preserve"> B26 - B27</f>
         <v>5415.4262499999995</v>
       </c>

</xml_diff>